<commit_message>
feat: streamline for loop to one for blankRowInserter.py
</commit_message>
<xml_diff>
--- a/Chap14_Excel-Spreadsheets/editBlank.xlsx
+++ b/Chap14_Excel-Spreadsheets/editBlank.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,73 +450,76 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>49405.53253472222</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Pears</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>49407.37480324074</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Oranges</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>49409.08819444444</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Apples</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>152</v>
-      </c>
-    </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>49409.75737268518</v>
+        <v>49405.53253472222</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Bananas</t>
+          <t>Pears</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
+        <v>49407.37480324074</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Oranges</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>49409.08819444444</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Apples</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>49409.75737268518</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Bananas</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
         <v>49409.11164351852</v>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B12" t="inlineStr">
         <is>
           <t>Strawberries</t>
         </is>
       </c>
-      <c r="C9" t="n">
+      <c r="C12" t="n">
         <v>98</v>
       </c>
     </row>
-    <row r="10"/>
-    <row r="11"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
+    <row r="16"/>
+    <row r="17"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>